<commit_message>
working on optimization of script
</commit_message>
<xml_diff>
--- a/excelFiles/TutorialsNinja.xlsx
+++ b/excelFiles/TutorialsNinja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zuber\PycharmProjects\SeleniumPythonHybridFrameWork\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447BBA42-AE54-47E7-9210-B6F03B7AFC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58117F2F-8F21-4570-AF19-F5123CEC38B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -34,25 +34,40 @@
     <t>Password</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
     <t>zubertest0@gmail.com</t>
   </si>
   <si>
     <t>zubertest0+01@gmail.com</t>
   </si>
   <si>
-    <t>zuber</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>01061997</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>user@.com</t>
+  </si>
+  <si>
+    <t>user@c.c</t>
+  </si>
+  <si>
+    <t>12#ab@com.c</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>user.gmail.com</t>
+  </si>
+  <si>
+    <t>user@gmail@gmail.com</t>
+  </si>
+  <si>
+    <t>user@c</t>
   </si>
 </sst>
 </file>
@@ -127,18 +142,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -422,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -442,18 +459,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -469,31 +486,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881A56EE-EDE1-4CA9-B455-9AAE669FBC69}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{174E9762-4B70-4C4B-9272-4882984F2924}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{BDC0AA35-8F6B-40F9-A850-C600C33175AD}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{AB89F2BB-AD35-465C-9315-489A06A5BFD4}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{5456334A-845F-4DFC-A153-A8D27FACA1C1}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{2EC41715-DB84-4B9C-9D07-491515856785}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>